<commit_message>
Updating with minor changes based on review
</commit_message>
<xml_diff>
--- a/downloads/development/Real Time Exemption Checking Service - Client RTM v1.3.xlsx
+++ b/downloads/development/Real Time Exemption Checking Service - Client RTM v1.3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hscic365.sharepoint.com/sites/etp Archive/Real Time Exemption Checking/RTEC Full Technical Specification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hscic365.sharepoint.com@SSL\DavWWWRoot\sites\etp Archive\Real Time Exemption Checking\RTEC Full Technical Specification\Final RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{45D456E6-A1FE-479A-A504-0574C7F5FD2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D0323F4-2DB6-49F2-B000-7AACC5D4E735}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{45D456E6-A1FE-479A-A504-0574C7F5FD2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFB111F1-6E71-4B02-BFAF-03256588F5AB}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{04827DCF-B668-234F-B339-2F85470C261F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{04827DCF-B668-234F-B339-2F85470C261F}"/>
   </bookViews>
   <sheets>
     <sheet name="Rx Exemption Checking - Funct" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="132">
   <si>
     <t>Requirement Reference</t>
   </si>
@@ -193,9 +193,6 @@
     <t>Systems must include prescription exemption checks in scope of the system audit log.</t>
   </si>
   <si>
-    <t>PEC-FR-45</t>
-  </si>
-  <si>
     <t>PEC-FR-49</t>
   </si>
   <si>
@@ -381,9 +378,6 @@
   </si>
   <si>
     <t>Systems must inform the user that they need not obtain evidence or an exemption declaration where a prescription exemption check has shown an exemption applies.</t>
-  </si>
-  <si>
-    <t>Systems must allow prompts for obtaining declaration and signature and token printing to be configurable as toggled on or off.</t>
   </si>
   <si>
     <t>Systems should allow printing of tokens for Schedule 2 &amp; 3 Controlled Drugs to be configurable as toggled on or off.</t>
@@ -867,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8181F2D2-CFC8-A34F-86A0-67A89DB2F62D}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -883,12 +877,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
@@ -910,7 +904,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -921,7 +915,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -976,7 +970,7 @@
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1042,7 +1036,7 @@
         <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1053,7 +1047,7 @@
         <v>27</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -1064,7 +1058,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1075,7 +1069,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -1130,7 +1124,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
@@ -1141,7 +1135,7 @@
         <v>39</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -1152,7 +1146,7 @@
         <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
@@ -1160,7 +1154,7 @@
         <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1204,7 +1198,7 @@
         <v>48</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -1215,7 +1209,7 @@
         <v>49</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1237,21 +1231,21 @@
         <v>52</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
         <v>53</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
@@ -1259,32 +1253,32 @@
         <v>55</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="47.25" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A38" t="s">
+      <c r="C38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A39" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="47.25" x14ac:dyDescent="0.5">
-      <c r="A39" t="s">
-        <v>107</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
@@ -1292,20 +1286,9 @@
         <v>57</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A41" t="s">
-        <v>58</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C41" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1333,12 +1316,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
@@ -1357,10 +1340,10 @@
     </row>
     <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1368,10 +1351,10 @@
     </row>
     <row r="6" spans="1:4" ht="78.75" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1379,10 +1362,10 @@
     </row>
     <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1390,10 +1373,10 @@
     </row>
     <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1401,10 +1384,10 @@
     </row>
     <row r="9" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -1412,21 +1395,21 @@
     </row>
     <row r="10" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A11" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -1434,10 +1417,10 @@
     </row>
     <row r="12" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -1445,10 +1428,10 @@
     </row>
     <row r="13" spans="1:4" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -1456,10 +1439,10 @@
     </row>
     <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -1467,21 +1450,21 @@
     </row>
     <row r="15" spans="1:4" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -1489,10 +1472,10 @@
     </row>
     <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -1500,10 +1483,10 @@
     </row>
     <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
@@ -1511,10 +1494,10 @@
     </row>
     <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A19" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
@@ -1522,10 +1505,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
@@ -1533,21 +1516,21 @@
     </row>
     <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A22" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -1555,10 +1538,10 @@
     </row>
     <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A23" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -1566,32 +1549,32 @@
     </row>
     <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A24" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -1599,10 +1582,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -1610,10 +1593,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1621,13 +1604,13 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" t="s">
         <v>105</v>
       </c>
-      <c r="B29" t="s">
-        <v>106</v>
-      </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1636,8 +1619,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B34DEAFFF43E44491565FE2BB1BEA91" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a274c25872d64957a5a610c90f092fa4">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c0b3723-ae66-45ac-94fb-aaf049c45b50" xmlns:ns3="855546ab-18f6-475b-a7ad-6260db2875ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c8a3da0571228171ea62aaa82f50cee9" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B34DEAFFF43E44491565FE2BB1BEA91" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e66f4cedec422a01270da5b494dfbbe8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c0b3723-ae66-45ac-94fb-aaf049c45b50" xmlns:ns3="855546ab-18f6-475b-a7ad-6260db2875ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="164d09562df0331be4cdeac0273da4f9" ns2:_="" ns3:_="">
     <xsd:import namespace="2c0b3723-ae66-45ac-94fb-aaf049c45b50"/>
     <xsd:import namespace="855546ab-18f6-475b-a7ad-6260db2875ec"/>
     <xsd:element name="properties">
@@ -1655,6 +1638,7 @@
                 <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1719,6 +1703,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -1824,6 +1813,27 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="2c0b3723-ae66-45ac-94fb-aaf049c45b50">NHSD2400-688874767-633</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="2c0b3723-ae66-45ac-94fb-aaf049c45b50">
+      <Url>https://hscic365.sharepoint.com/sites/etp%20Archive/_layouts/15/DocIdRedir.aspx?ID=NHSD2400-688874767-633</Url>
+      <Description>NHSD2400-688874767-633</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1873,50 +1883,23 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="2c0b3723-ae66-45ac-94fb-aaf049c45b50">NHSD2400-688874767-633</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="2c0b3723-ae66-45ac-94fb-aaf049c45b50">
-      <Url>https://hscic365.sharepoint.com/sites/etp%20Archive/_layouts/15/DocIdRedir.aspx?ID=NHSD2400-688874767-633</Url>
-      <Description>NHSD2400-688874767-633</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE4E4724-A70D-4E0D-9DFA-CCDFD29E6999}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2c0b3723-ae66-45ac-94fb-aaf049c45b50"/>
-    <ds:schemaRef ds:uri="855546ab-18f6-475b-a7ad-6260db2875ec"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF1671E2-0D3B-49B3-B3C2-E903326DF402}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{995C5FEF-B9B2-436A-B664-7F5A0EF1CE9A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F486C9FB-183B-4456-8FD5-C519F6B1CD8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="855546ab-18f6-475b-a7ad-6260db2875ec"/>
+    <ds:schemaRef ds:uri="2c0b3723-ae66-45ac-94fb-aaf049c45b50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1930,18 +1913,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F486C9FB-183B-4456-8FD5-C519F6B1CD8B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{995C5FEF-B9B2-436A-B664-7F5A0EF1CE9A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="855546ab-18f6-475b-a7ad-6260db2875ec"/>
-    <ds:schemaRef ds:uri="2c0b3723-ae66-45ac-94fb-aaf049c45b50"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>